<commit_message>
Centrale warmtepomp+boiler van warmtenet aangesloten op 'MS' niveau
Centrale warmtepomp+boiler van warmtenet aangesloten op 'MS' niveau, net als de centrale windmolen dus.
Energie-balans van warmtenet wordt nu vanuit main aangeroepen.
Primair energieverbruik van warmtenet wordt toegekend aan buurten, via warmtevraag van aangesloten huishoudens en efficientie van warmtenet.
</commit_message>
<xml_diff>
--- a/models/AlbatrossProcessedVehicleTrips.xlsx
+++ b/models/AlbatrossProcessedVehicleTrips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/p_hogeveen_tue_nl/Documents/Documents/GitHub/HOLON/models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{29B25285-D0E8-431A-A16E-B540AF1E5230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{611B8096-DA02-4FF0-8E6C-9ED72C39CDF8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D168EEB-D907-4C70-BBB9-5316E9253FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6017BC1-6FAF-4018-A039-DA80AEFB0BF2}"/>
+    <workbookView xWindow="14235" yWindow="2340" windowWidth="28815" windowHeight="18420" xr2:uid="{B6017BC1-6FAF-4018-A039-DA80AEFB0BF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -543,7 +543,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F214DC1-9D17-4C7E-A3B1-FE4A682CAE2E}">
   <dimension ref="A1:AX584"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:T7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -948,7 +950,7 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>378</v>
@@ -966,51 +968,42 @@
         <v>2277</v>
       </c>
       <c r="H7">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I7">
         <v>3449</v>
       </c>
       <c r="J7">
-        <v>3746</v>
+        <v>4092</v>
       </c>
       <c r="K7">
+        <v>336</v>
+      </c>
+      <c r="L7">
+        <v>4806</v>
+      </c>
+      <c r="M7">
+        <v>5075</v>
+      </c>
+      <c r="N7">
+        <v>45</v>
+      </c>
+      <c r="O7">
+        <v>6215</v>
+      </c>
+      <c r="P7">
+        <v>6863</v>
+      </c>
+      <c r="Q7">
         <v>20</v>
       </c>
-      <c r="L7">
-        <v>3751</v>
-      </c>
-      <c r="M7">
-        <v>4092</v>
-      </c>
-      <c r="N7">
-        <v>336</v>
-      </c>
-      <c r="O7">
-        <v>4806</v>
-      </c>
-      <c r="P7">
-        <v>5075</v>
-      </c>
-      <c r="Q7">
-        <v>45</v>
-      </c>
       <c r="R7">
-        <v>6215</v>
+        <v>7745</v>
       </c>
       <c r="S7">
-        <v>6863</v>
+        <v>7973</v>
       </c>
       <c r="T7">
-        <v>20</v>
-      </c>
-      <c r="U7">
-        <v>7745</v>
-      </c>
-      <c r="V7">
-        <v>7973</v>
-      </c>
-      <c r="W7">
         <v>25</v>
       </c>
     </row>

</xml_diff>